<commit_message>
feat(projet): Ajoute la détection des touches du clavier pressé
les touches détecter sont W, A, S et D
</commit_message>
<xml_diff>
--- a/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
+++ b/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\I-320\Projet\Local repo\Projet320-ShootEmUp\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04D9E63-9ADE-4FDE-BCF3-DD737D6BCF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2D7027-88EB-4800-B3FC-528A9DD7D085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="5835" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Auteur:</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>Push git hub</t>
+  </si>
+  <si>
+    <t>Revue des users story</t>
+  </si>
+  <si>
+    <t>Connaisances largement insuffisante pour coder</t>
+  </si>
+  <si>
+    <t>Ajout de la détection des keys press</t>
   </si>
 </sst>
 </file>
@@ -1180,10 +1189,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>470</c:v>
+                  <c:v>490</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2113,16 +2122,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.87037037037037035</c:v>
+                  <c:v>0.72058823529411764</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.17647058823529413</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12962962962962962</c:v>
+                  <c:v>0.10294117647058823</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4311,7 +4320,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4366,7 +4375,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>9 heures 0 minutes</v>
+        <v>11 heures 20 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4381,15 +4390,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>300</v>
+        <v>420</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>540</v>
+        <v>680</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4657,15 +4666,23 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="63" t="str">
+      <c r="A15" s="63">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="34"/>
+        <v>38</v>
+      </c>
+      <c r="B15" s="34">
+        <v>45917</v>
+      </c>
       <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="23"/>
+      <c r="D15" s="36">
+        <v>20</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="G15" s="40"/>
       <c r="N15">
         <v>8</v>
@@ -4675,16 +4692,28 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="str">
+      <c r="A16" s="62">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="39"/>
+        <v>38</v>
+      </c>
+      <c r="B16" s="30">
+        <v>45917</v>
+      </c>
+      <c r="C16" s="31">
+        <v>2</v>
+      </c>
+      <c r="D16" s="32">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>45</v>
+      </c>
       <c r="O16">
         <v>40</v>
       </c>
@@ -11033,11 +11062,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C10" si="0">SUM(A6:B6)</f>
-        <v>470</v>
+        <v>490</v>
       </c>
       <c r="E6" s="70" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11045,11 +11074,11 @@
       </c>
       <c r="F6" s="71" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>7 h 50 min</v>
+        <v>8 h 10 min</v>
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.87037037037037035</v>
+        <v>0.72058823529411764</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11066,7 +11095,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
@@ -11074,7 +11103,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11082,11 +11111,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
+        <v>2 h 00 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0</v>
+        <v>0.17647058823529413</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11160,7 +11189,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.12962962962962962</v>
+        <v>0.10294117647058823</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11212,26 +11241,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>300</v>
+        <v>420</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>540</v>
+        <v>680</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>9 h 00 min</v>
+        <v>11 h 20 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.10227272727272728</v>
+        <v>0.12878787878787878</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11275,6 +11304,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11284,15 +11322,6 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11509,6 +11538,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11517,14 +11554,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat(AirSpace): début d'implémentation du système de check avec le sol
</commit_message>
<xml_diff>
--- a/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
+++ b/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\I-320\Projet\Local repo\Projet320-ShootEmUp\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2D7027-88EB-4800-B3FC-528A9DD7D085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6291819F-BCC0-401F-AC0C-F88627848661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5835" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Auteur:</t>
   </si>
@@ -182,6 +182,15 @@
   </si>
   <si>
     <t>Ajout de la détection des keys press</t>
+  </si>
+  <si>
+    <t>Lecture de la théorie</t>
+  </si>
+  <si>
+    <t>Déplacement du joueur</t>
+  </si>
+  <si>
+    <t>Implémentation du check de colision avec le sol</t>
   </si>
 </sst>
 </file>
@@ -1189,10 +1198,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>490</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2122,16 +2131,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.72058823529411764</c:v>
+                  <c:v>0.69714285714285718</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17647058823529413</c:v>
+                  <c:v>0.22285714285714286</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10294117647058823</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4320,7 +4329,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4375,7 +4384,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>11 heures 20 minutes</v>
+        <v>14 heures 35 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4390,15 +4399,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>420</v>
+        <v>540</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>260</v>
+        <v>335</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>680</v>
+        <v>875</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4719,45 +4728,71 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="str">
+      <c r="A17" s="63">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="23"/>
+        <v>39</v>
+      </c>
+      <c r="B17" s="34">
+        <v>45924</v>
+      </c>
+      <c r="C17" s="35">
+        <v>2</v>
+      </c>
+      <c r="D17" s="36">
+        <v>0</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>47</v>
+      </c>
       <c r="G17" s="40"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="str">
+      <c r="A18" s="62">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="30"/>
+        <v>39</v>
+      </c>
+      <c r="B18" s="30">
+        <v>45924</v>
+      </c>
       <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="23"/>
+      <c r="D18" s="32">
+        <v>30</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>48</v>
+      </c>
       <c r="G18" s="39"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="str">
+      <c r="A19" s="63">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="34"/>
+        <v>39</v>
+      </c>
+      <c r="B19" s="34">
+        <v>45924</v>
+      </c>
       <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="23"/>
+      <c r="D19" s="36">
+        <v>45</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="G19" s="40"/>
       <c r="O19">
         <v>55</v>
@@ -11058,7 +11093,7 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>300</v>
+        <v>420</v>
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
@@ -11066,7 +11101,7 @@
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C10" si="0">SUM(A6:B6)</f>
-        <v>490</v>
+        <v>610</v>
       </c>
       <c r="E6" s="70" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11074,11 +11109,11 @@
       </c>
       <c r="F6" s="71" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>8 h 10 min</v>
+        <v>10 h 10 min</v>
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.72058823529411764</v>
+        <v>0.69714285714285718</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11099,11 +11134,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11111,11 +11146,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>2 h 00 min</v>
+        <v>3 h 15 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.17647058823529413</v>
+        <v>0.22285714285714286</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11189,7 +11224,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.10294117647058823</v>
+        <v>0.08</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11241,26 +11276,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>420</v>
+        <v>540</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>260</v>
+        <v>335</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>680</v>
+        <v>875</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>11 h 20 min</v>
+        <v>14 h 35 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.12878787878787878</v>
+        <v>0.16571969696969696</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11304,15 +11339,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11322,6 +11348,15 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11538,14 +11573,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11554,6 +11581,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
chore(ship, airspace):Changement du système pour bouger le joueur
</commit_message>
<xml_diff>
--- a/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
+++ b/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\I-320\Projet\Local repo\Projet320-ShootEmUp\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\I-320\Projet\Local repo\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6291819F-BCC0-401F-AC0C-F88627848661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEE220C-5470-4FEC-8DD1-ED4676555287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="5280" yWindow="585" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>Auteur:</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>Implémentation du check de colision avec le sol</t>
+  </si>
+  <si>
+    <t>Changement du système pour bouger le joueur</t>
+  </si>
+  <si>
+    <t>beaucoup de bug de l'editeur</t>
   </si>
 </sst>
 </file>
@@ -1201,7 +1207,7 @@
                   <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>195</c:v>
+                  <c:v>375</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2131,16 +2137,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.69714285714285718</c:v>
+                  <c:v>0.5781990521327014</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22285714285714286</c:v>
+                  <c:v>0.35545023696682465</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.08</c:v>
+                  <c:v>6.6350710900473939E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4327,9 +4333,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4384,7 +4390,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>14 heures 35 minutes</v>
+        <v>17 heures 35 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4399,7 +4405,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>540</v>
+        <v>720</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -4407,7 +4413,7 @@
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>875</v>
+        <v>1055</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4799,16 +4805,28 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="62" t="str">
+      <c r="A20" s="62">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="39"/>
+        <v>40</v>
+      </c>
+      <c r="B20" s="30">
+        <v>45931</v>
+      </c>
+      <c r="C20" s="31">
+        <v>3</v>
+      </c>
+      <c r="D20" s="32">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="str">
@@ -11113,7 +11131,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.69714285714285718</v>
+        <v>0.5781990521327014</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11130,7 +11148,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
@@ -11138,7 +11156,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>195</v>
+        <v>375</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11146,11 +11164,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>3 h 15 min</v>
+        <v>6 h 15 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.22285714285714286</v>
+        <v>0.35545023696682465</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11224,7 +11242,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.08</v>
+        <v>6.6350710900473939E-2</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11276,7 +11294,7 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>540</v>
+        <v>720</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
@@ -11284,18 +11302,18 @@
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>875</v>
+        <v>1055</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>14 h 35 min</v>
+        <v>17 h 35 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.16571969696969696</v>
+        <v>0.19981060606060605</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11339,6 +11357,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11348,15 +11375,6 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11573,6 +11591,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11581,14 +11607,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
doc(jdt): mise a jour du temps utiliser au 08.10.2025
</commit_message>
<xml_diff>
--- a/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
+++ b/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\I-320\Projet\Local repo\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEE220C-5470-4FEC-8DD1-ED4676555287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF4D28D-E6D2-42C6-A309-A79912986CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="585" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Auteur:</t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>beaucoup de bug de l'editeur</t>
+  </si>
+  <si>
+    <t>Retablissement du mouvement du vaisseau</t>
+  </si>
+  <si>
+    <t>Gestion des collisions avec les coté de la fenetre</t>
+  </si>
+  <si>
+    <t>Gestion des collisions avec le sol</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1216,7 @@
                   <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>375</c:v>
+                  <c:v>555</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2137,16 +2146,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.5781990521327014</c:v>
+                  <c:v>0.49392712550607287</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35545023696682465</c:v>
+                  <c:v>0.44939271255060731</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.6350710900473939E-2</c:v>
+                  <c:v>5.6680161943319839E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4333,9 +4342,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4390,7 +4399,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>17 heures 35 minutes</v>
+        <v>20 heures 35 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4405,15 +4414,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>720</v>
+        <v>840</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>335</v>
+        <v>395</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>1055</v>
+        <v>1235</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4829,39 +4838,65 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="str">
+      <c r="A21" s="63">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="34"/>
+        <v>41</v>
+      </c>
+      <c r="B21" s="34">
+        <v>45938</v>
+      </c>
       <c r="C21" s="35"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="23"/>
+      <c r="D21" s="36">
+        <v>30</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>52</v>
+      </c>
       <c r="G21" s="40"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="str">
+      <c r="A22" s="62">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="30"/>
+        <v>41</v>
+      </c>
+      <c r="B22" s="30">
+        <v>45938</v>
+      </c>
       <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="23"/>
+      <c r="D22" s="32">
+        <v>15</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="str">
+      <c r="A23" s="63">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="23"/>
+        <v>41</v>
+      </c>
+      <c r="B23" s="34">
+        <v>45938</v>
+      </c>
+      <c r="C23" s="35">
+        <v>2</v>
+      </c>
+      <c r="D23" s="36">
+        <v>15</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>54</v>
+      </c>
       <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -11131,7 +11166,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.5781990521327014</v>
+        <v>0.49392712550607287</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11148,15 +11183,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>300</v>
+        <v>420</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>375</v>
+        <v>555</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11164,11 +11199,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>6 h 15 min</v>
+        <v>9 h 15 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.35545023696682465</v>
+        <v>0.44939271255060731</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11242,7 +11277,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>6.6350710900473939E-2</v>
+        <v>5.6680161943319839E-2</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11294,26 +11329,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>720</v>
+        <v>840</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>335</v>
+        <v>395</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>1055</v>
+        <v>1235</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>17 h 35 min</v>
+        <v>20 h 35 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.19981060606060605</v>
+        <v>0.23390151515151514</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11357,15 +11392,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11375,6 +11401,15 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11591,14 +11626,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11607,6 +11634,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fixe(AirSpace.cs): Fixe du bug de out of memory causé par la non suppression d'objets après utilisation
</commit_message>
<xml_diff>
--- a/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
+++ b/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\I-320\Projet\Local repo\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E89643C-98AC-4610-A325-BB40B9923173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD9D612-07D7-46C3-B4F7-13B148CC6049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="7335" yWindow="2655" windowWidth="21570" windowHeight="12750" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>Auteur:</t>
   </si>
@@ -254,6 +254,12 @@
   </si>
   <si>
     <t>Tentative de regler un bug d'out of memory à cause des tirs qui surcharge la mémoire</t>
+  </si>
+  <si>
+    <t>Bug de out of memory regler</t>
+  </si>
+  <si>
+    <t>Forcer l'utilisation du GC</t>
   </si>
 </sst>
 </file>
@@ -1264,7 +1270,7 @@
                   <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1860</c:v>
+                  <c:v>1890</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2194,16 +2200,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.24015748031496062</c:v>
+                  <c:v>0.23735408560311283</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73228346456692917</c:v>
+                  <c:v>0.7354085603112841</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7559055118110236E-2</c:v>
+                  <c:v>2.7237354085603113E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4391,8 +4397,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G30" activeCellId="1" sqref="G41 G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4447,7 +4453,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>42 heures 20 minutes</v>
+        <v>42 heures 50 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4466,11 +4472,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>860</v>
+        <v>890</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>2540</v>
+        <v>2570</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5288,16 +5294,26 @@
       <c r="G39" s="40"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="62" t="str">
+      <c r="A40" s="62">
         <f>IF(ISBLANK(B40),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B40))</f>
-        <v/>
-      </c>
-      <c r="B40" s="30"/>
+        <v>43</v>
+      </c>
+      <c r="B40" s="30">
+        <v>45952</v>
+      </c>
       <c r="C40" s="31"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="39"/>
+      <c r="D40" s="32">
+        <v>30</v>
+      </c>
+      <c r="E40" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G40" s="39" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="63" t="str">
@@ -11362,7 +11378,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.24015748031496062</v>
+        <v>0.23735408560311283</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11383,11 +11399,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1860</v>
+        <v>1890</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11395,11 +11411,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>31 h 00 min</v>
+        <v>31 h 30 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.73228346456692917</v>
+        <v>0.7354085603112841</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11473,7 +11489,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>2.7559055118110236E-2</v>
+        <v>2.7237354085603113E-2</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11529,22 +11545,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>860</v>
+        <v>890</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>2540</v>
+        <v>2570</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>42 h 20 min</v>
+        <v>42 h 50 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.48106060606060608</v>
+        <v>0.48674242424242425</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11588,6 +11604,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11597,15 +11622,6 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11822,6 +11838,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11830,14 +11854,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
doc(Journal de Travail): mise a jour du journal au 22.10.2025
</commit_message>
<xml_diff>
--- a/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
+++ b/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\I-320\Projet\Local repo\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD9D612-07D7-46C3-B4F7-13B148CC6049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5F46A1-71F2-43BA-9B8E-C2D17D8F91D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7335" yWindow="2655" windowWidth="21570" windowHeight="12750" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="11400" yWindow="2745" windowWidth="27240" windowHeight="12750" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
   <si>
     <t>Auteur:</t>
   </si>
@@ -260,6 +260,27 @@
   </si>
   <si>
     <t>Forcer l'utilisation du GC</t>
+  </si>
+  <si>
+    <t>Séparation de la classe enemy et BasicEnemy</t>
+  </si>
+  <si>
+    <t>Ajout de la classe healBar pour pouvoir l'afficher sur toutes les entités</t>
+  </si>
+  <si>
+    <t>Ajout du système de collision et de dégats entre le joueur et les ennemis</t>
+  </si>
+  <si>
+    <t>Ajout du système de collision et de dégats entre le joueur et les tirs ennemies</t>
+  </si>
+  <si>
+    <t>Ajout du système de collision et de dégats entre les ennemies et les tirs du joueur</t>
+  </si>
+  <si>
+    <t>Lorsqu'un ennemie meurt, il a 1 chance sur 20 de lacher un item de soin</t>
+  </si>
+  <si>
+    <t>Déplacement des ennemies de type basique</t>
   </si>
 </sst>
 </file>
@@ -1270,7 +1291,7 @@
                   <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1890</c:v>
+                  <c:v>2145</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2200,16 +2221,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.23735408560311283</c:v>
+                  <c:v>0.21592920353982301</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7354085603112841</c:v>
+                  <c:v>0.75929203539823009</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7237354085603113E-2</c:v>
+                  <c:v>2.4778761061946902E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4397,8 +4418,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" activeCellId="1" sqref="G41 G30"/>
+      <pane ySplit="6" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4453,7 +4474,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>42 heures 50 minutes</v>
+        <v>47 heures 5 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4468,15 +4489,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>1680</v>
+        <v>1740</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>890</v>
+        <v>1085</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>2570</v>
+        <v>2825</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5316,87 +5337,145 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="63" t="str">
+      <c r="A41" s="63">
         <f>IF(ISBLANK(B41),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B41))</f>
-        <v/>
-      </c>
-      <c r="B41" s="34"/>
+        <v>43</v>
+      </c>
+      <c r="B41" s="34">
+        <v>45952</v>
+      </c>
       <c r="C41" s="35"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="22"/>
+      <c r="D41" s="36">
+        <v>45</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>73</v>
+      </c>
       <c r="G41" s="40"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="62" t="str">
+      <c r="A42" s="62">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v/>
-      </c>
-      <c r="B42" s="30"/>
+        <v>43</v>
+      </c>
+      <c r="B42" s="30">
+        <v>45952</v>
+      </c>
       <c r="C42" s="31"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="22"/>
+      <c r="D42" s="32">
+        <v>15</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="G42" s="39"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="63" t="str">
+      <c r="A43" s="63">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B43))</f>
-        <v/>
-      </c>
-      <c r="B43" s="34"/>
+        <v>43</v>
+      </c>
+      <c r="B43" s="34">
+        <v>45952</v>
+      </c>
       <c r="C43" s="35"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="22"/>
+      <c r="D43" s="36">
+        <v>35</v>
+      </c>
+      <c r="E43" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>75</v>
+      </c>
       <c r="G43" s="40"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="62" t="str">
+      <c r="A44" s="62">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B44))</f>
-        <v/>
-      </c>
-      <c r="B44" s="30"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="30">
+        <v>45952</v>
+      </c>
       <c r="C44" s="31"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="22"/>
+      <c r="D44" s="32">
+        <v>15</v>
+      </c>
+      <c r="E44" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>76</v>
+      </c>
       <c r="G44" s="39"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="63" t="str">
+      <c r="A45" s="63">
         <f>IF(ISBLANK(B45),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B45))</f>
-        <v/>
-      </c>
-      <c r="B45" s="34"/>
+        <v>43</v>
+      </c>
+      <c r="B45" s="34">
+        <v>45952</v>
+      </c>
       <c r="C45" s="35"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="22"/>
+      <c r="D45" s="36">
+        <v>30</v>
+      </c>
+      <c r="E45" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>77</v>
+      </c>
       <c r="G45" s="40"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="62" t="str">
+      <c r="A46" s="62">
         <f>IF(ISBLANK(B46),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B46))</f>
-        <v/>
-      </c>
-      <c r="B46" s="30"/>
+        <v>43</v>
+      </c>
+      <c r="B46" s="30">
+        <v>45952</v>
+      </c>
       <c r="C46" s="31"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="22"/>
+      <c r="D46" s="32">
+        <v>25</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>78</v>
+      </c>
       <c r="G46" s="39"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="63" t="str">
+      <c r="A47" s="63">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B47))</f>
-        <v/>
-      </c>
-      <c r="B47" s="34"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="22"/>
+        <v>43</v>
+      </c>
+      <c r="B47" s="34">
+        <v>45952</v>
+      </c>
+      <c r="C47" s="35">
+        <v>1</v>
+      </c>
+      <c r="D47" s="36">
+        <v>30</v>
+      </c>
+      <c r="E47" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="22" t="s">
+        <v>79</v>
+      </c>
       <c r="G47" s="40"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -11378,7 +11457,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.23735408560311283</v>
+        <v>0.21592920353982301</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11395,15 +11474,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>1260</v>
+        <v>1320</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>630</v>
+        <v>825</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1890</v>
+        <v>2145</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11411,11 +11490,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>31 h 30 min</v>
+        <v>35 h 45 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.7354085603112841</v>
+        <v>0.75929203539823009</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11489,7 +11568,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>2.7237354085603113E-2</v>
+        <v>2.4778761061946902E-2</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11541,26 +11620,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>1680</v>
+        <v>1740</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>890</v>
+        <v>1085</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>2570</v>
+        <v>2825</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>42 h 50 min</v>
+        <v>47 h 05 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.48674242424242425</v>
+        <v>0.53503787878787878</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
doc(Journal de Travail): Mise à jour du journal de travail au 24.10.2025
</commit_message>
<xml_diff>
--- a/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
+++ b/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\I-320\Projet\Local repo\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5F46A1-71F2-43BA-9B8E-C2D17D8F91D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9989DADF-B574-447A-98D2-CDC0B1472CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="2745" windowWidth="27240" windowHeight="12750" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="8445" yWindow="1485" windowWidth="27240" windowHeight="12750" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
   <si>
     <t>Auteur:</t>
   </si>
@@ -259,9 +259,6 @@
     <t>Bug de out of memory regler</t>
   </si>
   <si>
-    <t>Forcer l'utilisation du GC</t>
-  </si>
-  <si>
     <t>Séparation de la classe enemy et BasicEnemy</t>
   </si>
   <si>
@@ -281,6 +278,18 @@
   </si>
   <si>
     <t>Déplacement des ennemies de type basique</t>
+  </si>
+  <si>
+    <t>Ajout de la classe Missile, la possibilité  de tirer avec et les dégats sur les ennemies</t>
+  </si>
+  <si>
+    <t>Ajout de la classe MissileItem qui est un objet qui est ramassable par le joueur</t>
+  </si>
+  <si>
+    <t>Forcer l'utilisation du Garbage Collector, est ce une mauvaise pratique ?</t>
+  </si>
+  <si>
+    <t>Ajout des modèles des divers ennemies</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1300,7 @@
                   <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2145</c:v>
+                  <c:v>2295</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2221,16 +2230,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.21592920353982301</c:v>
+                  <c:v>0.20504201680672268</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75929203539823009</c:v>
+                  <c:v>0.77142857142857146</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4778761061946902E-2</c:v>
+                  <c:v>2.3529411764705882E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4419,7 +4428,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4474,7 +4483,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>47 heures 5 minutes</v>
+        <v>49 heures 35 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4489,15 +4498,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>1740</v>
+        <v>1800</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>1085</v>
+        <v>1175</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>2825</v>
+        <v>2975</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5333,7 +5342,7 @@
         <v>71</v>
       </c>
       <c r="G40" s="39" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -5352,7 +5361,7 @@
         <v>19</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G41" s="40"/>
     </row>
@@ -5372,7 +5381,7 @@
         <v>19</v>
       </c>
       <c r="F42" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G42" s="39"/>
     </row>
@@ -5392,7 +5401,7 @@
         <v>19</v>
       </c>
       <c r="F43" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G43" s="40"/>
     </row>
@@ -5412,7 +5421,7 @@
         <v>19</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G44" s="39"/>
     </row>
@@ -5432,7 +5441,7 @@
         <v>19</v>
       </c>
       <c r="F45" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G45" s="40"/>
     </row>
@@ -5452,7 +5461,7 @@
         <v>19</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G46" s="39"/>
     </row>
@@ -5474,44 +5483,70 @@
         <v>19</v>
       </c>
       <c r="F47" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G47" s="40"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="62">
+        <f>IF(ISBLANK(B48),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B48))</f>
+        <v>43</v>
+      </c>
+      <c r="B48" s="30">
+        <v>45953</v>
+      </c>
+      <c r="C48" s="31">
+        <v>1</v>
+      </c>
+      <c r="D48" s="32">
+        <v>45</v>
+      </c>
+      <c r="E48" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="G47" s="40"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="62" t="str">
-        <f>IF(ISBLANK(B48),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B48))</f>
-        <v/>
-      </c>
-      <c r="B48" s="30"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="22"/>
       <c r="G48" s="39"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="63" t="str">
+      <c r="A49" s="63">
         <f>IF(ISBLANK(B49),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B49))</f>
-        <v/>
-      </c>
-      <c r="B49" s="34"/>
+        <v>43</v>
+      </c>
+      <c r="B49" s="34">
+        <v>45953</v>
+      </c>
       <c r="C49" s="35"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="22"/>
+      <c r="D49" s="36">
+        <v>30</v>
+      </c>
+      <c r="E49" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="22" t="s">
+        <v>80</v>
+      </c>
       <c r="G49" s="40"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="62" t="str">
+      <c r="A50" s="62">
         <f>IF(ISBLANK(B50),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B50))</f>
-        <v/>
-      </c>
-      <c r="B50" s="30"/>
+        <v>43</v>
+      </c>
+      <c r="B50" s="30">
+        <v>45953</v>
+      </c>
       <c r="C50" s="31"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="22"/>
+      <c r="D50" s="32">
+        <v>15</v>
+      </c>
+      <c r="E50" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="22" t="s">
+        <v>82</v>
+      </c>
       <c r="G50" s="39"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -11457,7 +11492,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.21592920353982301</v>
+        <v>0.20504201680672268</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11474,15 +11509,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>1320</v>
+        <v>1380</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>825</v>
+        <v>915</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>2145</v>
+        <v>2295</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11490,11 +11525,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>35 h 45 min</v>
+        <v>38 h 15 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.75929203539823009</v>
+        <v>0.77142857142857146</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11568,7 +11603,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>2.4778761061946902E-2</v>
+        <v>2.3529411764705882E-2</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11620,26 +11655,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>1740</v>
+        <v>1800</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>1085</v>
+        <v>1175</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>2825</v>
+        <v>2975</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>47 h 05 min</v>
+        <v>49 h 35 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.53503787878787878</v>
+        <v>0.56344696969696972</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11683,15 +11718,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11701,6 +11727,15 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11917,14 +11952,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11933,6 +11960,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
doc(Journal de Travail): Mise à jour du journal de travail pour le 24.10.2025
</commit_message>
<xml_diff>
--- a/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
+++ b/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\I-320\Projet\Local repo\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9989DADF-B574-447A-98D2-CDC0B1472CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7D88D7-B81F-4F88-977C-E896EC1065E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8445" yWindow="1485" windowWidth="27240" windowHeight="12750" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="85">
   <si>
     <t>Auteur:</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>Ajout des modèles des divers ennemies</t>
+  </si>
+  <si>
+    <t>Ajout de la classe FrontEnemy, définition de son mouvement et de ses tirs</t>
+  </si>
+  <si>
+    <t>Ajout de la classe SniperEnemy, définition de ses tirs en fonction de ses mouvements et ajout de la collision de ses tirs avec le joueur</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1306,7 @@
                   <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2295</c:v>
+                  <c:v>2580</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2230,16 +2236,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.20504201680672268</c:v>
+                  <c:v>0.18711656441717792</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77142857142857146</c:v>
+                  <c:v>0.79141104294478526</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3529411764705882E-2</c:v>
+                  <c:v>2.1472392638036811E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4428,7 +4434,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4483,7 +4489,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>49 heures 35 minutes</v>
+        <v>54 heures 20 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4498,15 +4504,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>1800</v>
+        <v>2040</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>1175</v>
+        <v>1220</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>2975</v>
+        <v>3260</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5550,27 +5556,47 @@
       <c r="G50" s="39"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="63" t="str">
+      <c r="A51" s="63">
         <f>IF(ISBLANK(B51),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B51))</f>
-        <v/>
-      </c>
-      <c r="B51" s="34"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="22"/>
+        <v>43</v>
+      </c>
+      <c r="B51" s="34">
+        <v>45954</v>
+      </c>
+      <c r="C51" s="35">
+        <v>2</v>
+      </c>
+      <c r="D51" s="36">
+        <v>30</v>
+      </c>
+      <c r="E51" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="22" t="s">
+        <v>83</v>
+      </c>
       <c r="G51" s="40"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="62" t="str">
+      <c r="A52" s="62">
         <f>IF(ISBLANK(B52),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B52))</f>
-        <v/>
-      </c>
-      <c r="B52" s="30"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="22"/>
+        <v>43</v>
+      </c>
+      <c r="B52" s="30">
+        <v>45954</v>
+      </c>
+      <c r="C52" s="31">
+        <v>2</v>
+      </c>
+      <c r="D52" s="32">
+        <v>15</v>
+      </c>
+      <c r="E52" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>84</v>
+      </c>
       <c r="G52" s="39"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -11492,7 +11518,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.20504201680672268</v>
+        <v>0.18711656441717792</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11509,15 +11535,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>1380</v>
+        <v>1620</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>915</v>
+        <v>960</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>2295</v>
+        <v>2580</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11525,11 +11551,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>38 h 15 min</v>
+        <v>43 h 00 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.77142857142857146</v>
+        <v>0.79141104294478526</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11603,7 +11629,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>2.3529411764705882E-2</v>
+        <v>2.1472392638036811E-2</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11655,26 +11681,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>1800</v>
+        <v>2040</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>1175</v>
+        <v>1220</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>2975</v>
+        <v>3260</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>49 h 35 min</v>
+        <v>54 h 20 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.56344696969696972</v>
+        <v>0.61742424242424243</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Doc(journal de travail): mise à jour au 28.10.2025
</commit_message>
<xml_diff>
--- a/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
+++ b/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\I-320\Projet\Local repo\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\I-320\Projet\Local repo\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7D88D7-B81F-4F88-977C-E896EC1065E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC17BC5-37A6-43FD-A085-B564A3323243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8445" yWindow="1485" windowWidth="27240" windowHeight="12750" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
   <si>
     <t>Auteur:</t>
   </si>
@@ -296,6 +296,21 @@
   </si>
   <si>
     <t>Ajout de la classe SniperEnemy, définition de ses tirs en fonction de ses mouvements et ajout de la collision de ses tirs avec le joueur</t>
+  </si>
+  <si>
+    <t>Fix d'un bug, l'ennemie peut à nouveau toucher le joueur</t>
+  </si>
+  <si>
+    <t>Ajout de la classe Hud qui affiche le nombre de missile que possède le joueur</t>
+  </si>
+  <si>
+    <t>ajout du système de game over du joueur</t>
+  </si>
+  <si>
+    <t>Changement des noms des variables pour convenir aux conventions de nommage de l'ETML et ajout de commentaire aux endroits pertinant</t>
+  </si>
+  <si>
+    <t>Ajout d'une condition de victoire qui se produit à 2000 points</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1321,7 @@
                   <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2580</c:v>
+                  <c:v>2730</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1379,7 +1394,6 @@
     </c:legend>
     <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1387,6 +1401,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1752,7 +1767,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1760,6 +1774,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2236,16 +2251,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.18711656441717792</c:v>
+                  <c:v>0.17888563049853373</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.79141104294478526</c:v>
+                  <c:v>0.80058651026392957</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1472392638036811E-2</c:v>
+                  <c:v>2.0527859237536656E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2403,7 +2418,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2411,6 +2425,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4433,8 +4448,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+      <pane ySplit="6" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4489,7 +4504,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>54 heures 20 minutes</v>
+        <v>56 heures 50 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4508,11 +4523,11 @@
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>1220</v>
+        <v>1370</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>3260</v>
+        <v>3410</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5600,63 +5615,103 @@
       <c r="G52" s="39"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="63" t="str">
+      <c r="A53" s="63">
         <f>IF(ISBLANK(B53),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B53))</f>
-        <v/>
-      </c>
-      <c r="B53" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="B53" s="34">
+        <v>45958</v>
+      </c>
       <c r="C53" s="35"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="22"/>
+      <c r="D53" s="36">
+        <v>15</v>
+      </c>
+      <c r="E53" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>85</v>
+      </c>
       <c r="G53" s="40"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="62" t="str">
+      <c r="A54" s="62">
         <f>IF(ISBLANK(B54),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B54))</f>
-        <v/>
-      </c>
-      <c r="B54" s="30"/>
+        <v>44</v>
+      </c>
+      <c r="B54" s="30">
+        <v>45958</v>
+      </c>
       <c r="C54" s="31"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="22"/>
+      <c r="D54" s="32">
+        <v>45</v>
+      </c>
+      <c r="E54" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="G54" s="39"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="63" t="str">
+      <c r="A55" s="63">
         <f>IF(ISBLANK(B55),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B55))</f>
-        <v/>
-      </c>
-      <c r="B55" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="B55" s="34">
+        <v>45958</v>
+      </c>
       <c r="C55" s="35"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="22"/>
+      <c r="D55" s="36">
+        <v>45</v>
+      </c>
+      <c r="E55" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>87</v>
+      </c>
       <c r="G55" s="40"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="62" t="str">
+    <row r="56" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="62">
         <f>IF(ISBLANK(B56),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B56))</f>
-        <v/>
-      </c>
-      <c r="B56" s="30"/>
+        <v>44</v>
+      </c>
+      <c r="B56" s="30">
+        <v>45958</v>
+      </c>
       <c r="C56" s="31"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="39"/>
+      <c r="D56" s="32">
+        <v>30</v>
+      </c>
+      <c r="E56" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="39" t="s">
+        <v>88</v>
+      </c>
       <c r="G56" s="39"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="63" t="str">
+      <c r="A57" s="63">
         <f>IF(ISBLANK(B57),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B57))</f>
-        <v/>
-      </c>
-      <c r="B57" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="B57" s="34">
+        <v>45958</v>
+      </c>
       <c r="C57" s="35"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="40"/>
+      <c r="D57" s="36">
+        <v>15</v>
+      </c>
+      <c r="E57" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="40" t="s">
+        <v>89</v>
+      </c>
       <c r="G57" s="40"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -11518,7 +11573,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.18711656441717792</v>
+        <v>0.17888563049853373</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11539,11 +11594,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>960</v>
+        <v>1110</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>2580</v>
+        <v>2730</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11551,11 +11606,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>43 h 00 min</v>
+        <v>45 h 30 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.79141104294478526</v>
+        <v>0.80058651026392957</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11629,7 +11684,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>2.1472392638036811E-2</v>
+        <v>2.0527859237536656E-2</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11685,22 +11740,22 @@
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>1220</v>
+        <v>1370</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>3260</v>
+        <v>3410</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>54 h 20 min</v>
+        <v>56 h 50 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.61742424242424243</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11744,6 +11799,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11753,15 +11817,6 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11978,6 +12033,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11986,14 +12049,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
doc(journal de travail, Rapport): mise a jour du jdt et avancement dans le rapport
</commit_message>
<xml_diff>
--- a/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
+++ b/Doc/T-P_POO-gillhorset-JournalTravail.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\I-320\Projet\Local repo\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\I-320\Projet\Local Repo\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC17BC5-37A6-43FD-A085-B564A3323243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCE5363-7B43-4786-9B17-BD4D16C79391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="6675" yWindow="1410" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="92">
   <si>
     <t>Auteur:</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>Ajout d'une condition de victoire qui se produit à 2000 points</t>
+  </si>
+  <si>
+    <t>Conseption du diagramme UML</t>
+  </si>
+  <si>
+    <t>Conseption du rapport</t>
   </si>
 </sst>
 </file>
@@ -1327,7 +1333,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2251,16 +2257,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.17888563049853373</c:v>
+                  <c:v>0.17062937062937064</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80058651026392957</c:v>
+                  <c:v>0.76363636363636367</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0527859237536656E-2</c:v>
+                  <c:v>6.5734265734265732E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4448,8 +4454,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <pane ySplit="6" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4504,7 +4510,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>56 heures 50 minutes</v>
+        <v>59 heures 35 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4519,15 +4525,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>2040</v>
+        <v>2160</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>1370</v>
+        <v>1415</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>3410</v>
+        <v>3575</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5715,27 +5721,47 @@
       <c r="G57" s="40"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="62" t="str">
+      <c r="A58" s="62">
         <f>IF(ISBLANK(B58),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B58))</f>
-        <v/>
-      </c>
-      <c r="B58" s="30"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="39"/>
+        <v>44</v>
+      </c>
+      <c r="B58" s="30">
+        <v>45959</v>
+      </c>
+      <c r="C58" s="31">
+        <v>1</v>
+      </c>
+      <c r="D58" s="32">
+        <v>0</v>
+      </c>
+      <c r="E58" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="39" t="s">
+        <v>90</v>
+      </c>
       <c r="G58" s="39"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="63" t="str">
+      <c r="A59" s="63">
         <f>IF(ISBLANK(B59),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B59))</f>
-        <v/>
-      </c>
-      <c r="B59" s="34"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="40"/>
+        <v>44</v>
+      </c>
+      <c r="B59" s="34">
+        <v>45959</v>
+      </c>
+      <c r="C59" s="35">
+        <v>1</v>
+      </c>
+      <c r="D59" s="36">
+        <v>45</v>
+      </c>
+      <c r="E59" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="G59" s="40"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -11573,7 +11599,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.17888563049853373</v>
+        <v>0.17062937062937064</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11610,7 +11636,7 @@
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.80058651026392957</v>
+        <v>0.76363636363636367</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11664,15 +11690,15 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>235</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11680,11 +11706,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 10 min</v>
+        <v>3 h 55 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>2.0527859237536656E-2</v>
+        <v>6.5734265734265732E-2</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11736,26 +11762,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>2040</v>
+        <v>2160</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>1370</v>
+        <v>1415</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>3410</v>
+        <v>3575</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>56 h 50 min</v>
+        <v>59 h 35 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.64583333333333337</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11799,15 +11825,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11817,6 +11834,15 @@
     <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12033,14 +12059,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -12049,6 +12067,14 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>